<commit_message>
Add avionics CAD file
</commit_message>
<xml_diff>
--- a/ECAD/Asfaloth_L2_AVI/PCB_layout_causion.xlsx
+++ b/ECAD/Asfaloth_L2_AVI/PCB_layout_causion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asfaloth_L2\ECAD\Asfaloth_L2_AVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251825E5-EE3F-4CB4-8791-CE1A8D9E6E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70F42B1-39BC-4DEA-A00D-08D307E41948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBA9CB06-BD54-4971-BA42-52FFD2B72DBF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>grounding strategy</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -360,11 +360,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">JLCPCB AD gerber file convert </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.jlc.com/portal/server_guide_10171.html</t>
+    <t>I2C voltage level translation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/an/sbaa565/sbaa565.pdf?ts=1731703710758&amp;ref_url=https%253A%252F%252Fwww.google.com%252F</t>
+  </si>
+  <si>
+    <t>I2C layout suggestion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://blog.csdn.net/chenhuanqiangnihao/article/details/114027867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pullup resistors better place near MCU </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -766,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95499C1-4564-41E3-A90C-6528F2470B24}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -968,14 +979,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
@@ -999,131 +1015,134 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>11</v>
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>15</v>
+      <c r="A29" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" t="s">
-        <v>27</v>
+      <c r="A33" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" t="s">
-        <v>79</v>
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>82</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D42" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A29" r:id="rId1" xr:uid="{95FE1D29-CD66-4D19-8EB2-C04B44176714}"/>
+    <hyperlink ref="A33" r:id="rId1" xr:uid="{95FE1D29-CD66-4D19-8EB2-C04B44176714}"/>
     <hyperlink ref="E14" r:id="rId2" xr:uid="{002B7590-0AB4-4D22-A0A4-DB0DCEFA0000}"/>
     <hyperlink ref="D9" r:id="rId3" xr:uid="{F61B4F92-A5CB-482A-97E0-4D56C2E1DAA5}"/>
     <hyperlink ref="D14" r:id="rId4" xr:uid="{6D976B39-B6C4-4584-AA45-5892D83A95B8}"/>

</xml_diff>

<commit_message>
ADD ECAD and CAD
</commit_message>
<xml_diff>
--- a/ECAD/Asfaloth_L2_AVI/PCB_layout_causion.xlsx
+++ b/ECAD/Asfaloth_L2_AVI/PCB_layout_causion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asfaloth_L2\ECAD\Asfaloth_L2_AVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70F42B1-39BC-4DEA-A00D-08D307E41948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AB6038-9657-4EDE-A8F6-8E3E9E41E508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBA9CB06-BD54-4971-BA42-52FFD2B72DBF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
   <si>
     <t>grounding strategy</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -375,6 +375,58 @@
   </si>
   <si>
     <t xml:space="preserve">pullup resistors better place near MCU </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ver0. problem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C pullup resistor position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position better close to MCU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mti-7 DK header position not correct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1700mil-&gt;48.26mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Screw position blocked by LoRa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>put one LoRa in the middle of board</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tempurature sensor ADC forgot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C SDA SCL pullup resistor schematic false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only need one set pullup resistor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>terminal, DCDC, through hole PAD not show up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stm32, CAN controller,Top solder PAD not show up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -382,7 +434,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -407,13 +459,28 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -433,11 +500,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -775,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95499C1-4564-41E3-A90C-6528F2470B24}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1137,6 +1207,64 @@
       </c>
       <c r="D42" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish Asfaloth L2 avionics ver1.1
</commit_message>
<xml_diff>
--- a/ECAD/Asfaloth_L2_AVI/PCB_layout_causion.xlsx
+++ b/ECAD/Asfaloth_L2_AVI/PCB_layout_causion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asfaloth_L2\ECAD\Asfaloth_L2_AVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AB6038-9657-4EDE-A8F6-8E3E9E41E508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C444CEB5-63C1-46CF-B14F-2C4D8C95C766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBA9CB06-BD54-4971-BA42-52FFD2B72DBF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
   <si>
     <t>grounding strategy</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -427,6 +427,45 @@
   </si>
   <si>
     <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>final check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solder PAD and hole PAD show up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>top overlay check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ground, small broken island check after pour polygon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>top paste 有點不對, layout用藍色那層的不會裸露出來</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37pin D-sub確認固定孔位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVDD VDD用100uH磁珠連接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://blog.csdn.net/D_Katter/article/details/127743365</t>
+  </si>
+  <si>
+    <t>top/bottom paste, top/bottom solder check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -845,15 +884,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95499C1-4564-41E3-A90C-6528F2470B24}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="93.21875" bestFit="1" customWidth="1"/>
@@ -1201,6 +1240,14 @@
         <v>82</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" t="s">
+        <v>113</v>
+      </c>
+    </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>72</v>
@@ -1213,11 +1260,17 @@
       <c r="A45" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>100</v>
       </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
       <c r="C46" t="s">
         <v>101</v>
       </c>
@@ -1226,6 +1279,9 @@
       <c r="A47" t="s">
         <v>93</v>
       </c>
+      <c r="B47" t="s">
+        <v>104</v>
+      </c>
       <c r="C47" t="s">
         <v>94</v>
       </c>
@@ -1234,6 +1290,9 @@
       <c r="A48" t="s">
         <v>95</v>
       </c>
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
       <c r="C48" t="s">
         <v>96</v>
       </c>
@@ -1242,6 +1301,9 @@
       <c r="A49" t="s">
         <v>97</v>
       </c>
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
       <c r="C49" t="s">
         <v>98</v>
       </c>
@@ -1250,20 +1312,76 @@
       <c r="A50" t="s">
         <v>99</v>
       </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>